<commit_message>
worked on evalation excel files of getriebe and motor svm
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Motor/Ergebnisse_SVM_Motor.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Motor/Ergebnisse_SVM_Motor.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repositories\datascience_sensor_data\Maschinelles_Lernen\PythonClassifierApplication_Motor\PythonClassifierApplication\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git_repositories\datascience_sensor_data\Maschinelles_Lernen\PythonClassifierApplication_Motor\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
   <si>
     <t>lineare SVM</t>
   </si>
@@ -51,6 +51,21 @@
   </si>
   <si>
     <t>Accuracy</t>
+  </si>
+  <si>
+    <t>rbf SVM</t>
+  </si>
+  <si>
+    <t>accuracy</t>
+  </si>
+  <si>
+    <t>mean</t>
+  </si>
+  <si>
+    <t>Execution</t>
+  </si>
+  <si>
+    <t>std</t>
   </si>
 </sst>
 </file>
@@ -112,7 +127,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -130,6 +145,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -446,114 +469,326 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499BCC99-EC25-41F5-B124-71E260E06872}">
-  <dimension ref="A3:J6"/>
+  <dimension ref="A3:N51"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="6" max="6" width="13.28515625" style="3" customWidth="1"/>
-    <col min="7" max="10" width="13.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" style="3" customWidth="1"/>
+    <col min="8" max="11" width="13.28515625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="1"/>
+      <c r="G3" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="1"/>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="3">
+      <c r="F4" s="1"/>
+      <c r="G4" s="3">
         <v>100000</v>
       </c>
-      <c r="G4" s="2">
+      <c r="H4" s="2">
         <v>0.53652690000000003</v>
       </c>
-      <c r="H4" s="2">
+      <c r="I4" s="2">
         <v>0.75453139999999996</v>
       </c>
-      <c r="I4" s="2">
+      <c r="J4" s="2">
         <v>0.67832409999999999</v>
       </c>
-      <c r="J4" s="2">
-        <v>0.46347319999999997</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <f>C5+D5</f>
+      <c r="K4" s="2">
+        <f>1-H4</f>
+        <v>0.46347309999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C5">
+        <f>D5+E5</f>
         <v>420813</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>210406</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>210407</v>
       </c>
-      <c r="F5" s="5">
+      <c r="G5" s="5">
         <v>1</v>
       </c>
-      <c r="G5" s="6">
+      <c r="H5" s="6">
         <v>0.53690700000000002</v>
       </c>
-      <c r="H5" s="6">
+      <c r="I5" s="6">
         <v>0.75206879999999998</v>
       </c>
-      <c r="I5" s="6">
+      <c r="J5" s="6">
         <v>0.6740524</v>
       </c>
-      <c r="J5" s="6">
+      <c r="K5" s="6">
+        <f t="shared" ref="K5:K6" si="0">1-H5</f>
         <v>0.46309299999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="F6" s="3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G6" s="3">
         <v>1.0000000000000001E-5</v>
       </c>
-      <c r="G6" s="2">
+      <c r="H6" s="2">
         <v>0.53070479999999998</v>
       </c>
-      <c r="H6" s="2">
+      <c r="I6" s="2">
         <v>0.65746780000000005</v>
       </c>
-      <c r="I6" s="2">
+      <c r="J6" s="2">
         <v>0.59533849999999999</v>
       </c>
-      <c r="J6" s="2">
+      <c r="K6" s="2">
+        <f t="shared" si="0"/>
         <v>0.46929520000000002</v>
       </c>
     </row>
+    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="G8" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K8" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G9" s="10">
+        <v>1</v>
+      </c>
+      <c r="K9" s="2">
+        <f>1-H9</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G10" s="10">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2">
+        <v>0</v>
+      </c>
+      <c r="I10" s="2">
+        <v>0</v>
+      </c>
+      <c r="J10" s="2">
+        <v>0</v>
+      </c>
+      <c r="K10" s="2">
+        <f>1-H10</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G11" s="10">
+        <v>3</v>
+      </c>
+      <c r="K11" s="2">
+        <f t="shared" ref="K11:K13" si="1">1-H11</f>
+        <v>1</v>
+      </c>
+      <c r="M11" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="N11" s="8"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G12" s="10">
+        <v>4</v>
+      </c>
+      <c r="K12" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G13" s="10">
+        <v>5</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="M13" s="9" t="e">
+        <f>AVERAGE(H12:H16)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N13" t="e">
+        <f>_xlfn.STDEV.P(H12:H16)</f>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G14" s="10"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G15" s="10"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" s="10"/>
+    </row>
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G17" s="10"/>
+    </row>
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G18" s="10"/>
+    </row>
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G19" s="10"/>
+    </row>
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G20" s="10"/>
+    </row>
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G21" s="10"/>
+    </row>
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G22" s="10"/>
+    </row>
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G23" s="10"/>
+    </row>
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G24" s="10"/>
+    </row>
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G25" s="10"/>
+    </row>
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G26" s="10"/>
+    </row>
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G27" s="10"/>
+    </row>
+    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G28" s="10"/>
+    </row>
+    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G29" s="10"/>
+    </row>
+    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G30" s="10"/>
+    </row>
+    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G31" s="10"/>
+    </row>
+    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G32" s="10"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G33" s="10"/>
+    </row>
+    <row r="34" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G34" s="10"/>
+    </row>
+    <row r="35" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G35" s="10"/>
+    </row>
+    <row r="36" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G36" s="10"/>
+    </row>
+    <row r="37" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G37" s="10"/>
+    </row>
+    <row r="38" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G38" s="10"/>
+    </row>
+    <row r="39" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G39" s="10"/>
+    </row>
+    <row r="40" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G40" s="10"/>
+    </row>
+    <row r="41" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G41" s="10"/>
+    </row>
+    <row r="42" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G42" s="10"/>
+    </row>
+    <row r="43" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G43" s="10"/>
+    </row>
+    <row r="44" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G44" s="10"/>
+    </row>
+    <row r="45" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G45" s="10"/>
+    </row>
+    <row r="46" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G46" s="10"/>
+    </row>
+    <row r="47" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G47" s="10"/>
+    </row>
+    <row r="48" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G48" s="10"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="10"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="10"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="10"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="M11:N11"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
worked on evaluation metrics file of SVM motor
</commit_message>
<xml_diff>
--- a/Maschinelles_Lernen/PythonClassifierApplication_Motor/Ergebnisse_SVM_Motor.xlsx
+++ b/Maschinelles_Lernen/PythonClassifierApplication_Motor/Ergebnisse_SVM_Motor.xlsx
@@ -23,8 +23,48 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Martin Trat</author>
+  </authors>
+  <commentList>
+    <comment ref="D3" authorId="0" shapeId="0" xr:uid="{12295AF8-E9C2-4777-83D8-0929F3B33085}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin Trat
+wenige Werte werden evtl. wegen falscher Formatierung in Datenbank herausgefiltert</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D19" authorId="0" shapeId="0" xr:uid="{1BDB7744-7FF4-400E-9D8F-CDEB18246B09}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Segoe UI"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Martin Trat
+wenige Werte werden evtl. wegen falscher Formatierung in Datenbank herausgefiltert</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="16">
   <si>
     <t>lineare SVM</t>
   </si>
@@ -66,6 +106,12 @@
   </si>
   <si>
     <t>std</t>
+  </si>
+  <si>
+    <t>nicht normalisiert</t>
+  </si>
+  <si>
+    <t>(C=1)</t>
   </si>
 </sst>
 </file>
@@ -75,7 +121,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,6 +136,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Segoe UI"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -127,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -141,19 +194,29 @@
     <xf numFmtId="2" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -468,11 +531,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499BCC99-EC25-41F5-B124-71E260E06872}">
-  <dimension ref="A3:N51"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{499BCC99-EC25-41F5-B124-71E260E06872}">
+  <dimension ref="A3:N56"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+      <selection activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,7 +545,7 @@
   </cols>
   <sheetData>
     <row r="3" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -512,284 +575,533 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="3">
-        <v>100000</v>
+        <v>10000000</v>
       </c>
       <c r="H4" s="2">
-        <v>0.53652690000000003</v>
+        <v>0.5383329</v>
       </c>
       <c r="I4" s="2">
-        <v>0.75453139999999996</v>
+        <v>0.75114289999999995</v>
       </c>
       <c r="J4" s="2">
-        <v>0.67832409999999999</v>
+        <v>0.67276670000000005</v>
       </c>
       <c r="K4" s="2">
         <f>1-H4</f>
-        <v>0.46347309999999997</v>
+        <v>0.4616671</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="C5">
-        <f>D5+E5</f>
-        <v>420813</v>
+        <f>522805+529235</f>
+        <v>1052040</v>
       </c>
       <c r="D5">
-        <v>210406</v>
+        <f>D6*$C$5</f>
+        <v>105204</v>
       </c>
       <c r="E5">
-        <v>210407</v>
-      </c>
-      <c r="G5" s="5">
+        <f>E6*$C$5</f>
+        <v>210408</v>
+      </c>
+      <c r="G5" s="8">
+        <v>1.7</v>
+      </c>
+      <c r="H5" s="2">
+        <v>0.53816180000000002</v>
+      </c>
+      <c r="I5" s="2">
+        <v>0.75090800000000002</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.67334850000000002</v>
+      </c>
+      <c r="K5" s="2">
+        <f>1-H5</f>
+        <v>0.46183819999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="C6" s="9">
         <v>1</v>
       </c>
-      <c r="H5" s="6">
-        <v>0.53690700000000002</v>
-      </c>
-      <c r="I5" s="6">
-        <v>0.75206879999999998</v>
-      </c>
-      <c r="J5" s="6">
-        <v>0.6740524</v>
-      </c>
-      <c r="K5" s="6">
-        <f t="shared" ref="K5:K6" si="0">1-H5</f>
-        <v>0.46309299999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G6" s="3">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="H6" s="2">
-        <v>0.53070479999999998</v>
-      </c>
-      <c r="I6" s="2">
-        <v>0.65746780000000005</v>
-      </c>
-      <c r="J6" s="2">
-        <v>0.59533849999999999</v>
-      </c>
-      <c r="K6" s="2">
+      <c r="D6" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="G6" s="11">
+        <v>1</v>
+      </c>
+      <c r="H6" s="5">
+        <v>0.53694030000000004</v>
+      </c>
+      <c r="I6" s="5">
+        <v>0.75128649999999997</v>
+      </c>
+      <c r="J6" s="5">
+        <v>0.67553759999999996</v>
+      </c>
+      <c r="K6" s="5">
+        <f t="shared" ref="K6:K8" si="0">1-H6</f>
+        <v>0.46305969999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G7" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="H7" s="10">
+        <v>0.53721600000000003</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0.74706629999999996</v>
+      </c>
+      <c r="J7" s="10">
+        <v>0.67075779999999996</v>
+      </c>
+      <c r="K7" s="10">
         <f t="shared" si="0"/>
-        <v>0.46929520000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" ht="30" x14ac:dyDescent="0.25">
-      <c r="G8" s="4" t="s">
+        <v>0.46278399999999997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G8" s="3">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0.52755370000000001</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.63316410000000001</v>
+      </c>
+      <c r="J8" s="10">
+        <v>0.57682999999999995</v>
+      </c>
+      <c r="K8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.47244629999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="F10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H10" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I10" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J10" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K10" s="4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G9" s="10">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F11" s="14"/>
+      <c r="G11" s="8">
         <v>1</v>
       </c>
-      <c r="K9" s="2">
-        <f>1-H9</f>
+      <c r="H11" s="10">
+        <v>0.53694030000000004</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.75128649999999997</v>
+      </c>
+      <c r="J11" s="10">
+        <v>0.67553759999999996</v>
+      </c>
+      <c r="K11" s="10">
+        <f>1-H11</f>
+        <v>0.46305969999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F12" s="14"/>
+      <c r="G12" s="8">
+        <v>2</v>
+      </c>
+      <c r="H12" s="2">
+        <v>0.5374584</v>
+      </c>
+      <c r="I12" s="2">
+        <v>0.74940569999999995</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.67264159999999995</v>
+      </c>
+      <c r="K12" s="2">
+        <f>1-H12</f>
+        <v>0.4625416</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F13" s="14"/>
+      <c r="G13" s="8">
+        <v>3</v>
+      </c>
+      <c r="H13" s="2">
+        <v>0.53842789999999996</v>
+      </c>
+      <c r="I13" s="2">
+        <v>0.75630390000000003</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.67801350000000005</v>
+      </c>
+      <c r="K13" s="2">
+        <f t="shared" ref="K13:K15" si="1">1-H13</f>
+        <v>0.46157210000000004</v>
+      </c>
+      <c r="M13" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="N13" s="13"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F14" s="14"/>
+      <c r="G14" s="8">
+        <v>4</v>
+      </c>
+      <c r="H14" s="2">
+        <v>0.53769599999999995</v>
+      </c>
+      <c r="I14" s="2">
+        <v>0.75595440000000003</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.67664570000000002</v>
+      </c>
+      <c r="K14" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46230400000000005</v>
+      </c>
+      <c r="M14" t="s">
+        <v>11</v>
+      </c>
+      <c r="N14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F15" s="14"/>
+      <c r="G15" s="8">
+        <v>5</v>
+      </c>
+      <c r="H15" s="2">
+        <v>0.53844689999999995</v>
+      </c>
+      <c r="I15" s="2">
+        <v>0.74967019999999995</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.67037469999999999</v>
+      </c>
+      <c r="K15" s="2">
+        <f t="shared" si="1"/>
+        <v>0.46155310000000005</v>
+      </c>
+      <c r="M15" s="7">
+        <f>AVERAGE(H11:H15)</f>
+        <v>0.53779389999999994</v>
+      </c>
+      <c r="N15">
+        <f>_xlfn.STDEV.P(H11:H15)</f>
+        <v>5.795071388688544E-4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G16" s="8"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G17" s="8"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G18" s="8"/>
+    </row>
+    <row r="19" spans="1:14" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="K19" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="14"/>
+      <c r="G20" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G10" s="10">
+      <c r="H20" s="2">
+        <v>0.59602580000000005</v>
+      </c>
+      <c r="I20" s="2">
+        <v>0.63216640000000002</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.43979970000000002</v>
+      </c>
+      <c r="K20" s="2">
+        <f>1-H20</f>
+        <v>0.40397419999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D21">
+        <f>D22*$C$5</f>
+        <v>105204</v>
+      </c>
+      <c r="E21">
+        <f>E22*$C$5</f>
+        <v>210408</v>
+      </c>
+      <c r="F21" s="14"/>
+      <c r="G21" s="8">
         <v>2</v>
       </c>
-      <c r="H10" s="2">
-        <v>0</v>
-      </c>
-      <c r="I10" s="2">
-        <v>0</v>
-      </c>
-      <c r="J10" s="2">
-        <v>0</v>
-      </c>
-      <c r="K10" s="2">
-        <f>1-H10</f>
+      <c r="H21" s="2">
+        <v>0</v>
+      </c>
+      <c r="I21" s="2">
+        <v>0</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0</v>
+      </c>
+      <c r="K21" s="2">
+        <f>1-H21</f>
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G11" s="10">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D22" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="14"/>
+      <c r="G22" s="8">
         <v>3</v>
       </c>
-      <c r="K11" s="2">
-        <f t="shared" ref="K11:K13" si="1">1-H11</f>
+      <c r="H22" s="2">
+        <v>0</v>
+      </c>
+      <c r="I22" s="2">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0</v>
+      </c>
+      <c r="K22" s="2">
+        <f t="shared" ref="K22:K24" si="2">1-H22</f>
         <v>1</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="M22" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="8"/>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G12" s="10">
+      <c r="N22" s="13"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F23" s="14"/>
+      <c r="G23" s="8">
         <v>4</v>
       </c>
-      <c r="K12" s="2">
-        <f t="shared" si="1"/>
+      <c r="H23" s="2">
+        <v>0</v>
+      </c>
+      <c r="I23" s="2">
+        <v>0</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0</v>
+      </c>
+      <c r="K23" s="2">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M23" t="s">
         <v>11</v>
       </c>
-      <c r="N12" t="s">
+      <c r="N23" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G13" s="10">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F24" s="14"/>
+      <c r="G24" s="8">
         <v>5</v>
       </c>
-      <c r="K13" s="2">
-        <f t="shared" si="1"/>
+      <c r="H24" s="2">
+        <v>0</v>
+      </c>
+      <c r="I24" s="2">
+        <v>0</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0</v>
+      </c>
+      <c r="K24" s="2">
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="M13" s="9" t="e">
-        <f>AVERAGE(H12:H16)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="N13" t="e">
-        <f>_xlfn.STDEV.P(H12:H16)</f>
-        <v>#DIV/0!</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G14" s="10"/>
-    </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="G15" s="10"/>
-    </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G16" s="10"/>
-    </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G17" s="10"/>
-    </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G18" s="10"/>
-    </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G19" s="10"/>
-    </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G20" s="10"/>
-    </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G21" s="10"/>
-    </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G22" s="10"/>
-    </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G23" s="10"/>
-    </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G24" s="10"/>
-    </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G25" s="10"/>
-    </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G26" s="10"/>
-    </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G27" s="10"/>
-    </row>
-    <row r="28" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G28" s="10"/>
-    </row>
-    <row r="29" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G29" s="10"/>
-    </row>
-    <row r="30" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G30" s="10"/>
-    </row>
-    <row r="31" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G32" s="10"/>
+      <c r="M24" s="7">
+        <f>AVERAGE(H20:H24)</f>
+        <v>0.11920516</v>
+      </c>
+      <c r="N24">
+        <f>_xlfn.STDEV.P(H20:H24)</f>
+        <v>0.23841032000000004</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G25" s="8"/>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G26" s="8"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G27" s="8"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G28" s="8"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G29" s="8"/>
+    </row>
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G30" s="8"/>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G31" s="8"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="G32" s="8"/>
     </row>
     <row r="33" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G33" s="10"/>
+      <c r="G33" s="8"/>
     </row>
     <row r="34" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G34" s="10"/>
+      <c r="G34" s="8"/>
     </row>
     <row r="35" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G35" s="10"/>
+      <c r="G35" s="8"/>
     </row>
     <row r="36" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G36" s="10"/>
+      <c r="G36" s="8"/>
     </row>
     <row r="37" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G37" s="10"/>
+      <c r="G37" s="8"/>
     </row>
     <row r="38" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G38" s="10"/>
+      <c r="G38" s="8"/>
     </row>
     <row r="39" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G39" s="10"/>
+      <c r="G39" s="8"/>
     </row>
     <row r="40" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G40" s="10"/>
+      <c r="G40" s="8"/>
     </row>
     <row r="41" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G41" s="10"/>
+      <c r="G41" s="8"/>
     </row>
     <row r="42" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G42" s="10"/>
+      <c r="G42" s="8"/>
     </row>
     <row r="43" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G43" s="10"/>
+      <c r="G43" s="8"/>
     </row>
     <row r="44" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G44" s="10"/>
+      <c r="G44" s="8"/>
     </row>
     <row r="45" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G45" s="10"/>
+      <c r="G45" s="8"/>
     </row>
     <row r="46" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G46" s="10"/>
+      <c r="G46" s="8"/>
     </row>
     <row r="47" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G47" s="10"/>
+      <c r="G47" s="8"/>
     </row>
     <row r="48" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G48" s="10"/>
+      <c r="G48" s="8"/>
     </row>
     <row r="49" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G49" s="10"/>
+      <c r="G49" s="8"/>
     </row>
     <row r="50" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G50" s="10"/>
+      <c r="G50" s="8"/>
     </row>
     <row r="51" spans="7:7" x14ac:dyDescent="0.25">
-      <c r="G51" s="10"/>
+      <c r="G51" s="8"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="8"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="8"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="8"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="8"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="M11:N11"/>
+  <mergeCells count="4">
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M22:N22"/>
+    <mergeCell ref="F10:F15"/>
+    <mergeCell ref="F19:F24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>